<commit_message>
Started implementing Ioanna's new indics. TODO: refactoring fromAMECO()
</commit_message>
<xml_diff>
--- a/Ioanna's modified and added indicators.xlsx
+++ b/Ioanna's modified and added indicators.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eceuropaeu-my.sharepoint.com/personal/aleksander_rutkowski_ec_europa_eu/Documents/JAF2R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{F1AFBD5B-C3CA-4AF3-9209-3D62511E2BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2427057-08C1-4752-BA21-31B4DDF35FA5}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{F1AFBD5B-C3CA-4AF3-9209-3D62511E2BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17D3A236-5907-42FF-8297-4F3DA23E47B0}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18796" xr2:uid="{D7E04C1B-D49C-46FF-9382-CD8D9229EED1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="18796" activeTab="1" xr2:uid="{D7E04C1B-D49C-46FF-9382-CD8D9229EED1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$AU$24</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="368">
   <si>
     <t>JAF_KEY</t>
   </si>
@@ -795,9 +795,6 @@
     <t>['bd_9bd_sz_cl_r2',['nace_r2=B-S_X_K642','sizeclas=TOTAL','indic_sb=V16910']]</t>
   </si>
   <si>
-    <t>PA8.2.S4.</t>
-  </si>
-  <si>
     <t>PA8.2</t>
   </si>
   <si>
@@ -873,15 +870,6 @@
     <t>Real unit labour cost growth (% change from previous year)</t>
   </si>
   <si>
-    <t>AMECO7</t>
-  </si>
-  <si>
-    <t>AMECO7 / code QLCD</t>
-  </si>
-  <si>
-    <t>(b/a - 1)*100</t>
-  </si>
-  <si>
     <t>PA9.1 S1.</t>
   </si>
   <si>
@@ -1138,6 +1126,24 @@
   </si>
   <si>
     <t>added</t>
+  </si>
+  <si>
+    <t>PA8.2.S4._modified</t>
+  </si>
+  <si>
+    <t>PA8.2.S4._added</t>
+  </si>
+  <si>
+    <t>(a/b - 1)*100</t>
+  </si>
+  <si>
+    <t>['AMECO7',['CODE=QLCD']]</t>
+  </si>
+  <si>
+    <t>AMECO</t>
+  </si>
+  <si>
+    <t>['AMECO7',['CODE=QLCD'],-1]</t>
   </si>
 </sst>
 </file>
@@ -1190,10 +1196,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1493,18 +1495,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8557D1B-9DEA-4DEB-8F2C-9A3DAEF22EF1}">
-  <dimension ref="A1:AV65"/>
+  <dimension ref="A1:AV42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AH39" sqref="AH39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1650,7 +1655,7 @@
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B2" t="s">
         <v>47</v>
@@ -1718,7 +1723,7 @@
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
@@ -1786,7 +1791,7 @@
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
         <v>68</v>
@@ -1854,7 +1859,7 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
         <v>72</v>
@@ -1922,7 +1927,7 @@
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
@@ -1990,7 +1995,7 @@
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B7" t="s">
         <v>81</v>
@@ -2058,7 +2063,7 @@
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B8" t="s">
         <v>85</v>
@@ -2126,7 +2131,7 @@
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B9" t="s">
         <v>89</v>
@@ -2194,7 +2199,7 @@
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
         <v>95</v>
@@ -2262,7 +2267,7 @@
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" t="s">
         <v>98</v>
@@ -2330,7 +2335,7 @@
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B12" t="s">
         <v>102</v>
@@ -2401,7 +2406,7 @@
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B13" t="s">
         <v>109</v>
@@ -2472,7 +2477,7 @@
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B14" t="s">
         <v>112</v>
@@ -2543,7 +2548,7 @@
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B15" t="s">
         <v>115</v>
@@ -2614,7 +2619,7 @@
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B16" t="s">
         <v>119</v>
@@ -2685,7 +2690,7 @@
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B17" t="s">
         <v>122</v>
@@ -2756,7 +2761,7 @@
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B18" t="s">
         <v>125</v>
@@ -2821,7 +2826,7 @@
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B19" t="s">
         <v>131</v>
@@ -2886,7 +2891,7 @@
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B20" t="s">
         <v>134</v>
@@ -2948,7 +2953,7 @@
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B21" t="s">
         <v>140</v>
@@ -3010,7 +3015,7 @@
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B22" t="s">
         <v>145</v>
@@ -3078,7 +3083,7 @@
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B23" t="s">
         <v>149</v>
@@ -3143,7 +3148,7 @@
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B24" t="s">
         <v>154</v>
@@ -3214,7 +3219,7 @@
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B25" t="s">
         <v>161</v>
@@ -3282,7 +3287,7 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B26" t="s">
         <v>165</v>
@@ -3350,7 +3355,7 @@
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B27" t="s">
         <v>168</v>
@@ -3418,7 +3423,7 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B28" t="s">
         <v>171</v>
@@ -3486,7 +3491,7 @@
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s">
         <v>176</v>
@@ -3554,7 +3559,7 @@
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s">
         <v>179</v>
@@ -3622,7 +3627,7 @@
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B31" t="s">
         <v>182</v>
@@ -3693,7 +3698,7 @@
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B32" t="s">
         <v>190</v>
@@ -3770,7 +3775,7 @@
     </row>
     <row r="33" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B33" t="s">
         <v>200</v>
@@ -3841,7 +3846,7 @@
     </row>
     <row r="34" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B34" t="s">
         <v>205</v>
@@ -3915,7 +3920,7 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B35" t="s">
         <v>212</v>
@@ -3986,7 +3991,7 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B36" t="s">
         <v>218</v>
@@ -4057,7 +4062,7 @@
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B37" t="s">
         <v>221</v>
@@ -4128,7 +4133,7 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B38" t="s">
         <v>224</v>
@@ -4199,7 +4204,7 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B39" t="s">
         <v>227</v>
@@ -4264,7 +4269,7 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s">
         <v>234</v>
@@ -4329,7 +4334,7 @@
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B41" t="s">
         <v>239</v>
@@ -4406,16 +4411,16 @@
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B42" t="s">
+        <v>362</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" t="s">
         <v>251</v>
-      </c>
-      <c r="C42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" t="s">
-        <v>252</v>
       </c>
       <c r="F42" t="s">
         <v>146</v>
@@ -4448,965 +4453,25 @@
         <v>1</v>
       </c>
       <c r="X42" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y42" t="s">
         <v>253</v>
       </c>
-      <c r="Y42" t="s">
+      <c r="Z42" t="s">
         <v>254</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>255</v>
       </c>
       <c r="AA42" t="s">
         <v>92</v>
       </c>
       <c r="AB42" t="s">
+        <v>255</v>
+      </c>
+      <c r="AC42" t="s">
         <v>256</v>
-      </c>
-      <c r="AC42" t="s">
-        <v>257</v>
       </c>
       <c r="AD42" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>365</v>
-      </c>
-      <c r="B43" t="s">
-        <v>260</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" t="s">
-        <v>50</v>
-      </c>
-      <c r="K43" t="s">
-        <v>261</v>
-      </c>
-      <c r="V43">
-        <v>1</v>
-      </c>
-      <c r="W43" t="s">
-        <v>262</v>
-      </c>
-      <c r="Y43" t="s">
-        <v>263</v>
-      </c>
-      <c r="Z43" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA43" t="s">
-        <v>264</v>
-      </c>
-      <c r="AB43" t="s">
-        <v>265</v>
-      </c>
-      <c r="AC43" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>365</v>
-      </c>
-      <c r="B44" t="s">
-        <v>267</v>
-      </c>
-      <c r="C44" t="s">
-        <v>48</v>
-      </c>
-      <c r="E44" t="s">
-        <v>50</v>
-      </c>
-      <c r="K44" t="s">
-        <v>261</v>
-      </c>
-      <c r="V44">
-        <v>1</v>
-      </c>
-      <c r="W44" t="s">
-        <v>268</v>
-      </c>
-      <c r="Y44" t="s">
-        <v>263</v>
-      </c>
-      <c r="Z44" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA44" t="s">
-        <v>264</v>
-      </c>
-      <c r="AB44" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC44" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>365</v>
-      </c>
-      <c r="B45" t="s">
-        <v>270</v>
-      </c>
-      <c r="C45" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" t="s">
-        <v>50</v>
-      </c>
-      <c r="K45" t="s">
-        <v>261</v>
-      </c>
-      <c r="V45">
-        <v>1</v>
-      </c>
-      <c r="W45" t="s">
-        <v>271</v>
-      </c>
-      <c r="Y45" t="s">
-        <v>263</v>
-      </c>
-      <c r="Z45" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA45" t="s">
-        <v>272</v>
-      </c>
-      <c r="AB45" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC45" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>365</v>
-      </c>
-      <c r="B46" t="s">
-        <v>275</v>
-      </c>
-      <c r="C46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" t="s">
-        <v>50</v>
-      </c>
-      <c r="K46" t="s">
-        <v>261</v>
-      </c>
-      <c r="V46">
-        <v>3</v>
-      </c>
-      <c r="W46" t="s">
-        <v>276</v>
-      </c>
-      <c r="Y46" t="s">
-        <v>277</v>
-      </c>
-      <c r="Z46" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA46" t="s">
-        <v>278</v>
-      </c>
-      <c r="AF46" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="47" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>365</v>
-      </c>
-      <c r="B47" t="s">
-        <v>280</v>
-      </c>
-      <c r="C47" t="s">
-        <v>48</v>
-      </c>
-      <c r="E47" t="s">
-        <v>146</v>
-      </c>
-      <c r="I47" t="s">
-        <v>281</v>
-      </c>
-      <c r="K47" t="s">
-        <v>261</v>
-      </c>
-      <c r="W47" t="s">
-        <v>282</v>
-      </c>
-      <c r="X47" t="s">
-        <v>283</v>
-      </c>
-      <c r="Y47" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z47" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA47" t="s">
-        <v>285</v>
-      </c>
-      <c r="AC47" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>365</v>
-      </c>
-      <c r="B48" t="s">
-        <v>286</v>
-      </c>
-      <c r="C48" t="s">
-        <v>48</v>
-      </c>
-      <c r="E48" t="s">
-        <v>50</v>
-      </c>
-      <c r="K48" t="s">
-        <v>261</v>
-      </c>
-      <c r="W48" t="s">
-        <v>287</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA48" t="s">
-        <v>288</v>
-      </c>
-      <c r="AC48" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD48" t="s">
-        <v>289</v>
-      </c>
-      <c r="AG48" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>365</v>
-      </c>
-      <c r="B49" t="s">
-        <v>290</v>
-      </c>
-      <c r="K49" t="s">
-        <v>261</v>
-      </c>
-      <c r="W49" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z49" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>292</v>
-      </c>
-      <c r="AB49" t="s">
-        <v>293</v>
-      </c>
-      <c r="AC49" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD49" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG49" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>365</v>
-      </c>
-      <c r="B50" t="s">
-        <v>297</v>
-      </c>
-      <c r="E50" t="s">
-        <v>50</v>
-      </c>
-      <c r="K50" t="s">
-        <v>261</v>
-      </c>
-      <c r="W50" t="s">
-        <v>298</v>
-      </c>
-      <c r="X50" t="s">
-        <v>299</v>
-      </c>
-      <c r="Y50" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z50" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA50" t="s">
-        <v>295</v>
-      </c>
-      <c r="AB50" t="s">
-        <v>300</v>
-      </c>
-      <c r="AC50" t="s">
-        <v>296</v>
-      </c>
-      <c r="AD50" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE50" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>365</v>
-      </c>
-      <c r="B51" t="s">
-        <v>301</v>
-      </c>
-      <c r="E51" t="s">
-        <v>50</v>
-      </c>
-      <c r="K51" t="s">
-        <v>261</v>
-      </c>
-      <c r="W51" t="s">
-        <v>302</v>
-      </c>
-      <c r="X51" t="s">
-        <v>299</v>
-      </c>
-      <c r="Y51" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z51" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA51" t="s">
-        <v>295</v>
-      </c>
-      <c r="AB51" t="s">
-        <v>300</v>
-      </c>
-      <c r="AC51" t="s">
-        <v>296</v>
-      </c>
-      <c r="AD51" t="s">
-        <v>303</v>
-      </c>
-      <c r="AE51" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>365</v>
-      </c>
-      <c r="B52" t="s">
-        <v>304</v>
-      </c>
-      <c r="C52" t="s">
-        <v>48</v>
-      </c>
-      <c r="E52" t="s">
-        <v>50</v>
-      </c>
-      <c r="I52" t="s">
-        <v>281</v>
-      </c>
-      <c r="K52" t="s">
-        <v>261</v>
-      </c>
-      <c r="W52" t="s">
-        <v>305</v>
-      </c>
-      <c r="X52" t="s">
-        <v>306</v>
-      </c>
-      <c r="Y52" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA52" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB52" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC52" t="s">
-        <v>308</v>
-      </c>
-      <c r="AD52" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE52" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>365</v>
-      </c>
-      <c r="B53" t="s">
-        <v>310</v>
-      </c>
-      <c r="C53" t="s">
-        <v>48</v>
-      </c>
-      <c r="E53" t="s">
-        <v>50</v>
-      </c>
-      <c r="I53" t="s">
-        <v>281</v>
-      </c>
-      <c r="K53" t="s">
-        <v>261</v>
-      </c>
-      <c r="W53" t="s">
-        <v>311</v>
-      </c>
-      <c r="X53" t="s">
-        <v>306</v>
-      </c>
-      <c r="Y53" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z53" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA53" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB53" t="s">
-        <v>303</v>
-      </c>
-      <c r="AC53" t="s">
-        <v>308</v>
-      </c>
-      <c r="AD53" t="s">
-        <v>94</v>
-      </c>
-      <c r="AE53" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>365</v>
-      </c>
-      <c r="B54" t="s">
-        <v>313</v>
-      </c>
-      <c r="C54" t="s">
-        <v>48</v>
-      </c>
-      <c r="D54" t="s">
-        <v>228</v>
-      </c>
-      <c r="E54" t="s">
-        <v>314</v>
-      </c>
-      <c r="I54" t="s">
-        <v>281</v>
-      </c>
-      <c r="K54" t="s">
-        <v>53</v>
-      </c>
-      <c r="W54" t="s">
-        <v>315</v>
-      </c>
-      <c r="X54" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y54" t="s">
-        <v>316</v>
-      </c>
-      <c r="AA54" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB54" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC54" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD54" t="s">
-        <v>61</v>
-      </c>
-      <c r="AE54" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>365</v>
-      </c>
-      <c r="B55" t="s">
-        <v>318</v>
-      </c>
-      <c r="C55" t="s">
-        <v>48</v>
-      </c>
-      <c r="D55" t="s">
-        <v>319</v>
-      </c>
-      <c r="E55" t="s">
-        <v>50</v>
-      </c>
-      <c r="K55" t="s">
-        <v>261</v>
-      </c>
-      <c r="W55" t="s">
-        <v>320</v>
-      </c>
-      <c r="X55" t="s">
-        <v>312</v>
-      </c>
-      <c r="Y55" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA55" t="s">
-        <v>321</v>
-      </c>
-      <c r="AB55" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>365</v>
-      </c>
-      <c r="B56" t="s">
-        <v>323</v>
-      </c>
-      <c r="C56" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" t="s">
-        <v>319</v>
-      </c>
-      <c r="E56" t="s">
-        <v>50</v>
-      </c>
-      <c r="K56" t="s">
-        <v>261</v>
-      </c>
-      <c r="W56" t="s">
-        <v>324</v>
-      </c>
-      <c r="X56" t="s">
-        <v>325</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA56" t="s">
-        <v>326</v>
-      </c>
-      <c r="AB56" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC56" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>365</v>
-      </c>
-      <c r="B57" t="s">
-        <v>327</v>
-      </c>
-      <c r="C57" t="s">
-        <v>48</v>
-      </c>
-      <c r="D57" t="s">
-        <v>319</v>
-      </c>
-      <c r="E57" t="s">
-        <v>50</v>
-      </c>
-      <c r="K57" t="s">
-        <v>261</v>
-      </c>
-      <c r="W57" t="s">
-        <v>328</v>
-      </c>
-      <c r="X57" t="s">
-        <v>329</v>
-      </c>
-      <c r="Y57" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>330</v>
-      </c>
-      <c r="AB57" t="s">
-        <v>331</v>
-      </c>
-      <c r="AC57" t="s">
-        <v>332</v>
-      </c>
-      <c r="AD57" t="s">
-        <v>333</v>
-      </c>
-      <c r="AE57" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>365</v>
-      </c>
-      <c r="B58" t="s">
-        <v>251</v>
-      </c>
-      <c r="C58" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" t="s">
-        <v>252</v>
-      </c>
-      <c r="E58" t="s">
-        <v>314</v>
-      </c>
-      <c r="K58" t="s">
-        <v>261</v>
-      </c>
-      <c r="W58" t="s">
-        <v>335</v>
-      </c>
-      <c r="X58" t="s">
-        <v>336</v>
-      </c>
-      <c r="Y58" t="s">
-        <v>284</v>
-      </c>
-      <c r="AA58" t="s">
-        <v>364</v>
-      </c>
-      <c r="AB58" t="s">
-        <v>337</v>
-      </c>
-      <c r="AC58" t="s">
-        <v>338</v>
-      </c>
-      <c r="AD58" t="s">
-        <v>339</v>
-      </c>
-      <c r="AE58" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>365</v>
-      </c>
-      <c r="B59" t="s">
-        <v>341</v>
-      </c>
-      <c r="C59" t="s">
-        <v>48</v>
-      </c>
-      <c r="E59" t="s">
-        <v>50</v>
-      </c>
-      <c r="K59" t="s">
-        <v>261</v>
-      </c>
-      <c r="W59" t="s">
-        <v>342</v>
-      </c>
-      <c r="X59" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y59" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA59" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB59" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC59" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD59" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE59" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>365</v>
-      </c>
-      <c r="B60" t="s">
-        <v>344</v>
-      </c>
-      <c r="C60" t="s">
-        <v>48</v>
-      </c>
-      <c r="E60" t="s">
-        <v>50</v>
-      </c>
-      <c r="K60" t="s">
-        <v>261</v>
-      </c>
-      <c r="W60" t="s">
-        <v>345</v>
-      </c>
-      <c r="X60" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y60" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA60" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB60" t="s">
-        <v>303</v>
-      </c>
-      <c r="AC60" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD60" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE60" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>365</v>
-      </c>
-      <c r="B61" t="s">
-        <v>346</v>
-      </c>
-      <c r="C61" t="s">
-        <v>48</v>
-      </c>
-      <c r="E61" t="s">
-        <v>347</v>
-      </c>
-      <c r="K61" t="s">
-        <v>261</v>
-      </c>
-      <c r="W61" t="s">
-        <v>348</v>
-      </c>
-      <c r="X61" t="s">
-        <v>349</v>
-      </c>
-      <c r="Y61" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z61" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA61" t="s">
-        <v>350</v>
-      </c>
-      <c r="AB61" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC61" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD61" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>365</v>
-      </c>
-      <c r="B62" t="s">
-        <v>351</v>
-      </c>
-      <c r="C62" t="s">
-        <v>352</v>
-      </c>
-      <c r="E62" t="s">
-        <v>50</v>
-      </c>
-      <c r="K62" t="s">
-        <v>261</v>
-      </c>
-      <c r="W62" t="s">
-        <v>353</v>
-      </c>
-      <c r="X62" t="s">
-        <v>349</v>
-      </c>
-      <c r="Y62" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA62" t="s">
-        <v>350</v>
-      </c>
-      <c r="AB62" t="s">
-        <v>354</v>
-      </c>
-      <c r="AC62" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD62" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>365</v>
-      </c>
-      <c r="B63" t="s">
-        <v>355</v>
-      </c>
-      <c r="C63" t="s">
-        <v>48</v>
-      </c>
-      <c r="E63" t="s">
-        <v>50</v>
-      </c>
-      <c r="K63" t="s">
-        <v>261</v>
-      </c>
-      <c r="W63" t="s">
-        <v>356</v>
-      </c>
-      <c r="X63" t="s">
-        <v>357</v>
-      </c>
-      <c r="Y63" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z63" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA63" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB63" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC63" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD63" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE63" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>365</v>
-      </c>
-      <c r="B64" t="s">
-        <v>358</v>
-      </c>
-      <c r="C64" t="s">
-        <v>48</v>
-      </c>
-      <c r="E64" t="s">
-        <v>50</v>
-      </c>
-      <c r="K64" t="s">
-        <v>261</v>
-      </c>
-      <c r="W64" t="s">
-        <v>359</v>
-      </c>
-      <c r="X64" t="s">
-        <v>360</v>
-      </c>
-      <c r="Y64" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z64" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA64" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB64" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC64" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD64" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE64" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>365</v>
-      </c>
-      <c r="B65" t="s">
-        <v>361</v>
-      </c>
-      <c r="C65" t="s">
-        <v>48</v>
-      </c>
-      <c r="E65" t="s">
-        <v>50</v>
-      </c>
-      <c r="K65" t="s">
-        <v>261</v>
-      </c>
-      <c r="W65" t="s">
-        <v>362</v>
-      </c>
-      <c r="X65" t="s">
-        <v>363</v>
-      </c>
-      <c r="Y65" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z65" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA65" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB65" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC65" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD65" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE65" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -5416,53 +4481,1108 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A61B30-A9EF-4268-B77E-06568805692D}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DC13F4D-D37A-4573-B7C1-83AFE5B8C8DD}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AU24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B1:B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" t="s">
+        <v>260</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>262</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>264</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K3" t="s">
+        <v>260</v>
+      </c>
+      <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>262</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>268</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" t="s">
+        <v>260</v>
+      </c>
+      <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>270</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>262</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>271</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" t="s">
+        <v>260</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
+      <c r="W5" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>366</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>364</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>365</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>361</v>
+      </c>
+      <c r="B6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>146</v>
+      </c>
+      <c r="I6" t="s">
+        <v>277</v>
+      </c>
+      <c r="K6" t="s">
+        <v>260</v>
+      </c>
+      <c r="W6" t="s">
+        <v>278</v>
+      </c>
+      <c r="X6" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>281</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
+        <v>260</v>
+      </c>
+      <c r="W7" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>285</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8" t="s">
+        <v>286</v>
+      </c>
+      <c r="K8" t="s">
+        <v>260</v>
+      </c>
+      <c r="W8" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>288</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>289</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>361</v>
+      </c>
+      <c r="B9" t="s">
+        <v>293</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" t="s">
+        <v>260</v>
+      </c>
+      <c r="W9" t="s">
+        <v>294</v>
+      </c>
+      <c r="X9" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>292</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>361</v>
+      </c>
+      <c r="B10" t="s">
+        <v>297</v>
+      </c>
+      <c r="E10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" t="s">
+        <v>260</v>
+      </c>
+      <c r="W10" t="s">
+        <v>298</v>
+      </c>
+      <c r="X10" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>291</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>292</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" t="s">
+        <v>300</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" t="s">
+        <v>277</v>
+      </c>
+      <c r="K11" t="s">
+        <v>260</v>
+      </c>
+      <c r="W11" t="s">
+        <v>301</v>
+      </c>
+      <c r="X11" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>303</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>304</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>361</v>
+      </c>
+      <c r="B12" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s">
+        <v>277</v>
+      </c>
+      <c r="K12" t="s">
+        <v>260</v>
+      </c>
+      <c r="W12" t="s">
+        <v>307</v>
+      </c>
+      <c r="X12" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>303</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>304</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>361</v>
+      </c>
+      <c r="B13" t="s">
+        <v>309</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E13" t="s">
+        <v>310</v>
+      </c>
+      <c r="I13" t="s">
+        <v>277</v>
+      </c>
+      <c r="K13" t="s">
+        <v>53</v>
+      </c>
+      <c r="W13" t="s">
+        <v>311</v>
+      </c>
+      <c r="X13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>312</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" t="s">
+        <v>314</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" t="s">
+        <v>260</v>
+      </c>
+      <c r="W14" t="s">
+        <v>316</v>
+      </c>
+      <c r="X14" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>317</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>315</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" t="s">
+        <v>260</v>
+      </c>
+      <c r="W15" t="s">
+        <v>320</v>
+      </c>
+      <c r="X15" t="s">
+        <v>321</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>361</v>
+      </c>
+      <c r="B16" t="s">
+        <v>323</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>315</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" t="s">
+        <v>260</v>
+      </c>
+      <c r="W16" t="s">
+        <v>324</v>
+      </c>
+      <c r="X16" t="s">
+        <v>325</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>361</v>
+      </c>
+      <c r="B17" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>251</v>
+      </c>
+      <c r="E17" t="s">
+        <v>310</v>
+      </c>
+      <c r="K17" t="s">
+        <v>260</v>
+      </c>
+      <c r="W17" t="s">
+        <v>331</v>
+      </c>
+      <c r="X17" t="s">
+        <v>332</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>360</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>333</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>334</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" t="s">
+        <v>260</v>
+      </c>
+      <c r="W18" t="s">
+        <v>338</v>
+      </c>
+      <c r="X18" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>361</v>
+      </c>
+      <c r="B19" t="s">
+        <v>340</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" t="s">
+        <v>260</v>
+      </c>
+      <c r="W19" t="s">
+        <v>341</v>
+      </c>
+      <c r="X19" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>361</v>
+      </c>
+      <c r="B20" t="s">
+        <v>342</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>343</v>
+      </c>
+      <c r="K20" t="s">
+        <v>260</v>
+      </c>
+      <c r="W20" t="s">
+        <v>344</v>
+      </c>
+      <c r="X20" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21" t="s">
+        <v>347</v>
+      </c>
+      <c r="C21" t="s">
+        <v>348</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" t="s">
+        <v>260</v>
+      </c>
+      <c r="W21" t="s">
+        <v>349</v>
+      </c>
+      <c r="X21" t="s">
+        <v>345</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>361</v>
+      </c>
+      <c r="B22" t="s">
+        <v>351</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" t="s">
+        <v>260</v>
+      </c>
+      <c r="W22" t="s">
+        <v>352</v>
+      </c>
+      <c r="X22" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>361</v>
+      </c>
+      <c r="B23" t="s">
+        <v>354</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" t="s">
+        <v>260</v>
+      </c>
+      <c r="W23" t="s">
+        <v>355</v>
+      </c>
+      <c r="X23" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>361</v>
+      </c>
+      <c r="B24" t="s">
+        <v>357</v>
+      </c>
+      <c r="C24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>50</v>
+      </c>
+      <c r="K24" t="s">
+        <v>260</v>
+      </c>
+      <c r="W24" t="s">
+        <v>358</v>
+      </c>
+      <c r="X24" t="s">
+        <v>359</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AU24" xr:uid="{6DC13F4D-D37A-4573-B7C1-83AFE5B8C8DD}">
+    <filterColumn colId="25">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194FB9B3-5EA6-4AF1-9E8B-605D1AFEC972}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EF06BD-DDAC-4485-AC19-54A35EFAEEC4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA540041-D4E8-48C7-906A-A9C19BFAE45A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>